<commit_message>
add level flight cpg control.
</commit_message>
<xml_diff>
--- a/自研飞控.xlsx
+++ b/自研飞控.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PPTFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF4B375-2747-4383-B567-D0375BD6A55C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7C865A-D1E2-4509-8396-10708ADD5908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{827C1629-CCAE-46AC-8959-6DB6873A2D9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{827C1629-CCAE-46AC-8959-6DB6873A2D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="硬件" sheetId="1" r:id="rId1"/>
@@ -511,18 +511,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>PWM输入</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>红色</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>PPM输入</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>4Hz闪烁</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -556,6 +548,14 @@
   </si>
   <si>
     <t>反转输入通道，从低位起第i位为1表示翻转第i个通道</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>平飞模式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>悬停模式</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A59B82B-0FAA-4EA9-83C3-D28EDF669906}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1355,7 +1355,7 @@
         <v>118</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="20"/>
@@ -1375,10 +1375,10 @@
         <v>3</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="10"/>
@@ -1398,10 +1398,10 @@
         <v>3</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="11"/>
@@ -1421,10 +1421,10 @@
         <v>3</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1441,10 +1441,10 @@
         <v>78</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1842,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B317485-1860-4B17-BF58-CD2C46D3D825}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2100,16 +2100,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>